<commit_message>
📊 Update announcements - 2026-02-03
</commit_message>
<xml_diff>
--- a/output/India_Corporate_Announcements_20260203.xlsx
+++ b/output/India_Corporate_Announcements_20260203.xlsx
@@ -42,7 +42,7 @@
       <sz val="14"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -59,12 +59,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFEB9C"/>
         <bgColor rgb="00FFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C6EFCE"/>
-        <bgColor rgb="00C6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -86,7 +80,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -95,9 +89,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -467,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,7 +471,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Indian Corporate Announcements Summary</t>
         </is>
@@ -489,12 +480,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Generated: 03 February 2026 10:42 AM</t>
+          <t>Generated: 03 February 2026 03:36 PM</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Announcements by Category</t>
         </is>
@@ -503,41 +494,41 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Investment</t>
+          <t>Board Meeting</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Order Win</t>
+          <t>Financial Results</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -547,160 +538,170 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Concall Transcript</t>
+          <t>Acquisition</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Dividend</t>
+          <t>Expansion</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="inlineStr">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Merger/Demerger</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Concall Transcript</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="inlineStr">
         <is>
           <t>Investment Implications Breakdown</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>★★★</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>★★</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="inlineStr">
+      <c r="B17" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="inlineStr">
         <is>
           <t>Companies with Most Announcements</t>
         </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>PG Electroplast Ltd</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Veronica Production Ltd</t>
+          <t>Lloyds Metals and Energy Ltd</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Oswal Pumps Ltd</t>
+          <t>Rashi Peripherals Ltd</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>National Fertilizers Ltd</t>
+          <t>Adf Foods Ltd-$</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Orient Press Ltd</t>
+          <t>Sterling Tools Ltd-$</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>The New India Assurance Company Ltd</t>
+          <t>Hari Govind International Ltd</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Seshasayee Paper and Boards Ltd</t>
+          <t>Trualt Bioenergy Ltd</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>UltraTech Cement Ltd</t>
+          <t>Bajaj Finance Ltd</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Castrol India Ltd</t>
+          <t>Expleo Solutions Ltd</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Wockhardt Ltd</t>
+          <t>Suzlon Energy Ltd</t>
         </is>
       </c>
       <c r="B29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Bank of Maharashtra</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
         <v>1</v>
       </c>
     </row>
@@ -785,20 +786,20 @@
     <row r="2" ht="80" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Orient Press Ltd</t>
+          <t>Suzlon Energy Ltd</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>526325</v>
+        <v>532667</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Orient Press Ltd - 526325 - Board Meeting Intimation for The Approval Of Unaudited Financial Results.</t>
+          <t>Suzlon Energy Ltd - 532667 - Rumour verification - Regulation 30(11)</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -808,12 +809,12 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>04:12 PM</t>
+          <t>09:04 PM</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>• Orient Press Ltd - 526325 - Board Meeting Intimation for The Approval Of Unaudited Financial Results</t>
+          <t>• Suzlon Energy Ltd - 532667 - Rumour verification - Regulation 30(11)</t>
         </is>
       </c>
       <c r="H2" s="3" t="inlineStr">
@@ -823,27 +824,27 @@
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/1526f511-c386-4f22-908d-708822e9c03a.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/db1380d5-f9ee-4b0c-a14e-cb2c2692bbdf.pdf</t>
         </is>
       </c>
     </row>
     <row r="3" ht="80" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>The New India Assurance Company Ltd</t>
+          <t>Lloyds Metals and Energy Ltd</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>540769</v>
+        <v>512455</v>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Investment</t>
+          <t>Acquisition</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>The New India Assurance Company Ltd - 540769 - Announcement under Regulation 30 (LODR)-Investor Presentation</t>
+          <t>Lloyds Metals and Energy Ltd - 512455 - Announcement under Regulation 30 (LODR)-Acquisition</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
@@ -853,33 +854,33 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>04:12 PM</t>
+          <t>09:03 PM</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>• The New India Assurance Company Ltd - 540769 - Announcement under Regulation 30 (LODR)-Investor Presentation</t>
+          <t>• Lloyds Metals and Energy Ltd - 512455 - Announcement under Regulation 30 (LODR)-Acquisition</t>
         </is>
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>★★ NEUTRAL</t>
+          <t>★★ MODERATE POSITIVE</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/a25900b7-aac9-4f56-bf82-76f647dd9a19.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/0afd6f5e-9705-4291-a3db-784ad4bf92a0.pdf</t>
         </is>
       </c>
     </row>
     <row r="4" ht="80" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Seshasayee Paper and Boards Ltd</t>
+          <t>Rashi Peripherals Ltd</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>502450</v>
+        <v>544119</v>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
@@ -888,7 +889,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Seshasayee Paper and Boards Ltd - 502450 - Announcement under Regulation 30 (LODR)-Newspaper Publication</t>
+          <t>Rashi Peripherals Ltd - 544119 - Intimation Of Formation Of Step-Down Subsidiary Company.</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
@@ -898,12 +899,12 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>04:12 PM</t>
+          <t>09:01 PM</t>
         </is>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>• Seshasayee Paper and Boards Ltd - 502450 - Announcement under Regulation 30 (LODR)-Newspaper Publication</t>
+          <t>• Rashi Peripherals Ltd - 544119 - Intimation Of Formation Of Step-Down Subsidiary Company</t>
         </is>
       </c>
       <c r="H4" s="3" t="inlineStr">
@@ -913,27 +914,27 @@
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/32e628cd-2b84-48ba-ab5d-874e8ecebff4.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/287697c2-789b-4f54-965b-2f8496982baa.pdf</t>
         </is>
       </c>
     </row>
     <row r="5" ht="80" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>UltraTech Cement Ltd</t>
+          <t>Adf Foods Ltd-$</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>532538</v>
+        <v>519183</v>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Order Win</t>
+          <t>Financial Results</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>UltraTech Cement Ltd - 532538 - Disclosure W.R.T. Orders Passed By GST Authority</t>
+          <t>Adf Foods Ltd-$ - 519183 - Unaudited Standalone And Consolidated Financial Results For The Quarter And Nine Months Ended 31St December, 2025.</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
@@ -943,42 +944,42 @@
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>04:11 PM</t>
+          <t>09:01 PM</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>• UltraTech Cement Ltd - 532538 - Disclosure W</t>
+          <t>• Adf Foods Ltd-$ - 519183 - Unaudited Standalone And Consolidated Financial Results For The Quarter And Nine Months Ended 31St December, 2025</t>
         </is>
       </c>
       <c r="H5" s="3" t="inlineStr">
         <is>
-          <t>★★ MODERATE POSITIVE</t>
+          <t>★★ NEUTRAL</t>
         </is>
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/94e62578-caed-435e-afde-a564e8609a30.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/737dbb96-e565-437a-89ca-9de4010cdbc6.pdf</t>
         </is>
       </c>
     </row>
     <row r="6" ht="80" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Castrol India Ltd</t>
+          <t>Sterling Tools Ltd-$</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>500870</v>
+        <v>530759</v>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>Castrol India Ltd - 500870 - Board Meeting Outcome for Outcome Of The Board Meeting Held On 3 February 2026.</t>
+          <t>Sterling Tools Ltd-$ - 530759 - Announcement under Regulation 30 (LODR)-Allotment of ESOP / ESPS</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
@@ -988,12 +989,12 @@
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>04:11 PM</t>
+          <t>09:00 PM</t>
         </is>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>• Castrol India Ltd - 500870 - Board Meeting Outcome for Outcome Of The Board Meeting Held On 3 February 2026</t>
+          <t>• Sterling Tools Ltd-$ - 530759 - Announcement under Regulation 30 (LODR)-Allotment of ESOP / ESPS</t>
         </is>
       </c>
       <c r="H6" s="3" t="inlineStr">
@@ -1003,27 +1004,27 @@
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/ac9f6dc2-2b65-4539-ba45-1e115041936f.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/f7844524-8ef5-4534-b290-18e5f8057ea2.pdf</t>
         </is>
       </c>
     </row>
     <row r="7" ht="80" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Veronica Production Ltd</t>
+          <t>Bank of Maharashtra</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>531695</v>
+        <v>532525</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Change in Directors</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>Veronica Production Ltd - 531695 - For December 31, 2025</t>
+          <t>Bank of Maharashtra - 532525 - Announcement under Regulation 30 (LODR)-Change in Directorate</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
@@ -1033,12 +1034,12 @@
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>04:10 PM</t>
+          <t>09:00 PM</t>
         </is>
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>• Veronica Production Ltd - 531695 - For December 31, 2025</t>
+          <t>• Bank of Maharashtra - 532525 - Announcement under Regulation 30 (LODR)-Change in Directorate</t>
         </is>
       </c>
       <c r="H7" s="3" t="inlineStr">
@@ -1048,27 +1049,27 @@
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/3612122a-29ea-4dcf-a609-f45653191196.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/7d34f006-d5ca-4246-ad0b-9341ca65a771.pdf</t>
         </is>
       </c>
     </row>
     <row r="8" ht="80" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Wockhardt Ltd</t>
+          <t>Trualt Bioenergy Ltd</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>532300</v>
+        <v>544545</v>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Financial Results</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>Wockhardt Ltd - 532300 - Announcement under Regulation 30 (LODR)-Change in Management</t>
+          <t>Trualt Bioenergy Ltd - 544545 - Consolidated And Standalone Unaudited Financial Results For The Quarter And Nine Months Ended December 31, 2025</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
@@ -1078,12 +1079,12 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>04:10 PM</t>
+          <t>08:59 PM</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>• Wockhardt Ltd - 532300 - Announcement under Regulation 30 (LODR)-Change in Management</t>
+          <t>• Trualt Bioenergy Ltd - 544545 - Consolidated And Standalone Unaudited Financial Results For The Quarter And Nine Months Ended December 31, 2025</t>
         </is>
       </c>
       <c r="H8" s="3" t="inlineStr">
@@ -1093,27 +1094,27 @@
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/8b65fabd-603b-4c9f-9fb6-4657182ac1ab.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/7ed30bcf-6620-4b8d-b17e-b2497a804aa6.pdf</t>
         </is>
       </c>
     </row>
     <row r="9" ht="80" customHeight="1">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>PG Electroplast Ltd</t>
+          <t>Lloyds Metals and Energy Ltd</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>533581</v>
+        <v>512455</v>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Investment</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>PG Electroplast Ltd - 533581 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
+          <t>Lloyds Metals and Energy Ltd - 512455 - Announcement under Regulation 30 (LODR)-Allotment</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
@@ -1123,12 +1124,12 @@
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>04:10 PM</t>
+          <t>08:56 PM</t>
         </is>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>• PG Electroplast Ltd - 533581 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
+          <t>• Lloyds Metals and Energy Ltd - 512455 - Announcement under Regulation 30 (LODR)-Allotment</t>
         </is>
       </c>
       <c r="H9" s="3" t="inlineStr">
@@ -1138,27 +1139,27 @@
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/82dd7d45-7c86-4045-9a17-dc3810e50fd6.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/ef9ea454-2167-4b93-ba15-f6c475a37583.pdf</t>
         </is>
       </c>
     </row>
     <row r="10" ht="80" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Scan Projects Ltd</t>
+          <t>Action Construction Equipment Ltd</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>531797</v>
+        <v>532762</v>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Financial Results</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>Scan Projects Ltd - 531797 - Board Meeting Intimation for Approve, Adopt And Consider Unaudited Financial Results For The Quarter Ended 31.12.2025.</t>
+          <t>Action Construction Equipment Ltd - 532762 - Earnings Presentation-Q3/9M-FY26</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
@@ -1168,12 +1169,12 @@
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>04:09 PM</t>
+          <t>08:53 PM</t>
         </is>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>• Scan Projects Ltd - 531797 - Board Meeting Intimation for Approve, Adopt And Consider Unaudited Financial Results For The Quarter Ended 31</t>
+          <t>• Action Construction Equipment Ltd - 532762 - Earnings Presentation-Q3/9M-FY26</t>
         </is>
       </c>
       <c r="H10" s="3" t="inlineStr">
@@ -1183,28 +1184,27 @@
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/de3d8a48-f048-4377-978e-d9de93b8d9ce.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/1bfb6273-d8cb-470d-bc81-9f8e2fb1112b.pdf</t>
         </is>
       </c>
     </row>
     <row r="11" ht="80" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>Biogen Pharmachem Industries Ltd</t>
+          <t>Max Estates Ltd</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>531752</v>
+        <v>544008</v>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Board Meeting</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Biogen Pharmachem Industries Ltd - 531752 - Updation Of Website Of The Company.
-</t>
+          <t>Max Estates Ltd - 544008 - Board Meeting Intimation for Prior Intimation - Board Meeting For Consideration Of Unaudited Financial Results Of The Company For The Quarter And Nine Months Ended December 31, 2025.</t>
         </is>
       </c>
       <c r="E11" s="2" t="inlineStr">
@@ -1214,12 +1214,12 @@
       </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
-          <t>04:09 PM</t>
+          <t>08:52 PM</t>
         </is>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
-          <t>• Biogen Pharmachem Industries Ltd - 531752 - Updation Of Website Of The Company</t>
+          <t>• Max Estates Ltd - 544008 - Board Meeting Intimation for Prior Intimation - Board Meeting For Consideration Of Unaudited Financial Results Of The Company For The Quarter And Nine Months Ended December 31, 2025</t>
         </is>
       </c>
       <c r="H11" s="3" t="inlineStr">
@@ -1229,18 +1229,18 @@
       </c>
       <c r="I11" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/41a09852-6242-4c8e-a650-2e9a790492f5.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/e3638f7e-24ea-4ca4-a365-e98aa3f07239.pdf</t>
         </is>
       </c>
     </row>
     <row r="12" ht="80" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>Calcom Vision Ltd</t>
+          <t>Adf Foods Ltd-$</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>517236</v>
+        <v>519183</v>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>Calcom Vision Ltd - 517236 - Board Meeting Intimation for Prior Intimation Of Board Meeting For Financial Results.</t>
+          <t>Adf Foods Ltd-$ - 519183 - Board Meeting Outcome for Board Meeting Held Today I.E. On Tuesday, 3Rd February, 2026.</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
@@ -1259,12 +1259,13 @@
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>04:08 PM</t>
+          <t>08:51 PM</t>
         </is>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>• Calcom Vision Ltd - 517236 - Board Meeting Intimation for Prior Intimation Of Board Meeting For Financial Results</t>
+          <t>• Adf Foods Ltd-$ - 519183 - Board Meeting Outcome for Board Meeting Held Today I
+• On Tuesday, 3Rd February, 2026</t>
         </is>
       </c>
       <c r="H12" s="3" t="inlineStr">
@@ -1274,18 +1275,18 @@
       </c>
       <c r="I12" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/07510737-d77e-4cd8-b5ad-680aff6051f1.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/7707eacf-e848-4ed0-9e7d-44f3d58ebdc2.pdf</t>
         </is>
       </c>
     </row>
     <row r="13" ht="80" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Varun Beverages Ltd</t>
+          <t>Nexus Select Trust</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>540180</v>
+        <v>543913</v>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
@@ -1294,7 +1295,7 @@
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Varun Beverages Ltd - 540180 - Announcement under Regulation 30 (LODR)-Allotment of ESOP / ESPS</t>
+          <t>Nexus Select Trust - 543913 - Reg 23(5)(i): Disclosure of material issue</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
@@ -1304,42 +1305,42 @@
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>04:08 PM</t>
+          <t>08:51 PM</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>• Varun Beverages Ltd - 540180 - Announcement under Regulation 30 (LODR)-Allotment of ESOP / ESPS</t>
+          <t>• Nexus Select Trust - 543913 - Reg 23(5)(i): Disclosure of material issue</t>
         </is>
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>★★ NEUTRAL</t>
+          <t>★★ WATCH</t>
         </is>
       </c>
       <c r="I13" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/447caf6f-6a9a-40a7-b4ea-640223bda57a.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/43d4d1c5-3011-4358-98ab-ccc44aec9934.pdf</t>
         </is>
       </c>
     </row>
     <row r="14" ht="80" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>Morepen Laboratories Ltd</t>
+          <t>Bajaj Finance Ltd</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>500288</v>
+        <v>500034</v>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>Morepen Laboratories Ltd - 500288 - Board Meeting Intimation for Q3-FY 26 Unaudited Financial Results</t>
+          <t>Bajaj Finance Ltd - 500034 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Outcome</t>
         </is>
       </c>
       <c r="E14" s="2" t="inlineStr">
@@ -1349,12 +1350,12 @@
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>04:08 PM</t>
+          <t>08:48 PM</t>
         </is>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>• Morepen Laboratories Ltd - 500288 - Board Meeting Intimation for Q3-FY 26 Unaudited Financial Results</t>
+          <t>• Bajaj Finance Ltd - 500034 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Outcome</t>
         </is>
       </c>
       <c r="H14" s="3" t="inlineStr">
@@ -1364,27 +1365,27 @@
       </c>
       <c r="I14" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/32018fd2-2e65-4af3-b52c-e12901d98a85.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/6a612a82-50ce-484c-93a9-a370237bf342.pdf</t>
         </is>
       </c>
     </row>
     <row r="15" ht="80" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>De Nora India Ltd</t>
+          <t>Ashok Leyland Ltd</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>590031</v>
+        <v>500477</v>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>De Nora India Ltd - 590031 - Board Meeting Outcome for Outcome Of Board Meeting Held On Tuesday, February 3, 2026</t>
+          <t>Ashok Leyland Ltd - 500477 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
@@ -1394,12 +1395,12 @@
       </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>04:07 PM</t>
+          <t>08:48 PM</t>
         </is>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>• De Nora India Ltd - 590031 - Board Meeting Outcome for Outcome Of Board Meeting Held On Tuesday, February 3, 2026</t>
+          <t>• Ashok Leyland Ltd - 500477 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
         </is>
       </c>
       <c r="H15" s="3" t="inlineStr">
@@ -1409,27 +1410,27 @@
       </c>
       <c r="I15" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/3f1ad0ae-c74e-4976-a473-97497a7a3f8e.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/75b87287-05c4-428f-b2b3-76950378d641.pdf</t>
         </is>
       </c>
     </row>
     <row r="16" ht="80" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>Veronica Production Ltd</t>
+          <t>Bajaj Finance Ltd</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>531695</v>
+        <v>500034</v>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>Veronica Production Ltd - 531695 - Board Meeting Outcome for Outcome Of Board Meeting Held Today I.E., February 3, 2026</t>
+          <t>Bajaj Finance Ltd - 500034 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Outcome</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
@@ -1439,12 +1440,12 @@
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>04:06 PM</t>
+          <t>08:47 PM</t>
         </is>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>• Veronica Production Ltd - 531695 - Board Meeting Outcome for Outcome Of Board Meeting Held Today I</t>
+          <t>• Bajaj Finance Ltd - 500034 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Outcome</t>
         </is>
       </c>
       <c r="H16" s="3" t="inlineStr">
@@ -1454,27 +1455,27 @@
       </c>
       <c r="I16" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/f3a12ab8-c66a-4cfb-9660-e4dac607109b.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/70662a7a-9ca6-4fe8-970e-1117ba5954c2.pdf</t>
         </is>
       </c>
     </row>
     <row r="17" ht="80" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>Oswal Pumps Ltd</t>
+          <t>Rashi Peripherals Ltd</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>544418</v>
+        <v>544119</v>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Investment</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>Oswal Pumps Ltd - 544418 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
+          <t>Rashi Peripherals Ltd - 544119 - Announcement under Regulation 30 (LODR)-Change in Management</t>
         </is>
       </c>
       <c r="E17" s="2" t="inlineStr">
@@ -1484,12 +1485,12 @@
       </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>04:06 PM</t>
+          <t>08:47 PM</t>
         </is>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>• Oswal Pumps Ltd - 544418 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
+          <t>• Rashi Peripherals Ltd - 544119 - Announcement under Regulation 30 (LODR)-Change in Management</t>
         </is>
       </c>
       <c r="H17" s="3" t="inlineStr">
@@ -1499,27 +1500,27 @@
       </c>
       <c r="I17" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/34bb313a-4b1e-4ced-8944-8f2c910a12e5.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/d3315b18-2b06-4ee2-bb28-3df082c44c49.pdf</t>
         </is>
       </c>
     </row>
     <row r="18" ht="80" customHeight="1">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>Indian Toners &amp; Developers Ltd-$</t>
+          <t>NTPC Green Energy Ltd</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>523586</v>
+        <v>544289</v>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>Change in Directors</t>
+          <t>Expansion</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>Indian Toners &amp; Developers Ltd-$ - 523586 - Announcement under Regulation 30 (LODR)-Resignation of Chief Financial Officer (CFO)</t>
+          <t>NTPC Green Energy Ltd - 544289 - NTPC Green Energy Limited Has Informed The Exchange About Declaration Of Commercial Operation Of Second Part Capacity Of 125 MW Out Of 500 MW Bhadla Solar PV Project Located In Rajasthan Of NTPC Renewable Energy Limited, A Wholly Owned Subsidiary Of NTPC Green Energy Limited W.E.F. 31.01.2026.</t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
@@ -1529,42 +1530,42 @@
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>04:05 PM</t>
+          <t>08:47 PM</t>
         </is>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>• Indian Toners &amp; Developers Ltd-$ - 523586 - Announcement under Regulation 30 (LODR)-Resignation of Chief Financial Officer (CFO)</t>
+          <t>• NTPC Green Energy Ltd - 544289 - NTPC Green Energy Limited Has Informed The Exchange About Declaration Of Commercial Operation Of Second Part Capacity Of 125 MW Out Of 500 MW Bhadla Solar PV Project Located In Rajasthan Of NTPC Renewable Energy Limited, A Wholly Owned Subsidiary Of NTPC Green Energy Limited W</t>
         </is>
       </c>
       <c r="H18" s="3" t="inlineStr">
         <is>
-          <t>★★ WATCH</t>
+          <t>★★ MODERATE POSITIVE</t>
         </is>
       </c>
       <c r="I18" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/39327740-a6ac-4ffb-8e60-1fe87cd63738.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/33720d00-b139-4a28-9e3f-b9bd7f5bb0ea.pdf</t>
         </is>
       </c>
     </row>
     <row r="19" ht="80" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>Classic Electricals Ltd</t>
+          <t>Lloyds Metals and Energy Ltd</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>512213</v>
+        <v>512455</v>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>Classic Electricals Ltd - 512213 - Board Meeting Intimation for Considering And Approving Inter Alia The Standalone Un-Audited Financial Results Of The Company For The Quarter And Nine Months Ended 31St December, 2025</t>
+          <t>Lloyds Metals and Energy Ltd - 512455 - Announcement under Regulation 30 (LODR)-Investor Presentation</t>
         </is>
       </c>
       <c r="E19" s="2" t="inlineStr">
@@ -1574,12 +1575,12 @@
       </c>
       <c r="F19" s="2" t="inlineStr">
         <is>
-          <t>04:04 PM</t>
+          <t>08:46 PM</t>
         </is>
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
-          <t>• Classic Electricals Ltd - 512213 - Board Meeting Intimation for Considering And Approving Inter Alia The Standalone Un-Audited Financial Results Of The Company For The Quarter And Nine Months Ended 31St December, 2025</t>
+          <t>• Lloyds Metals and Energy Ltd - 512455 - Announcement under Regulation 30 (LODR)-Investor Presentation</t>
         </is>
       </c>
       <c r="H19" s="3" t="inlineStr">
@@ -1589,18 +1590,18 @@
       </c>
       <c r="I19" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/0063f42d-d726-48b3-b05a-effa96991d6e.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/fdae9240-df9d-4cc6-8fee-ddb633cf9b2f.pdf</t>
         </is>
       </c>
     </row>
     <row r="20" ht="80" customHeight="1">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>Shalibhadra Finance Ltd</t>
+          <t>Sri Lotus Developers and Realty Ltd</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>511754</v>
+        <v>544469</v>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
@@ -1609,7 +1610,7 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>Shalibhadra Finance Ltd - 511754 - Board Meeting Intimation for Intimation Of Board Meeting.</t>
+          <t>Sri Lotus Developers and Realty Ltd - 544469 - Board Meeting Intimation for Consideration Of Un-Audited (Standalone And Consolidated) Financial Results For The Quarter And Nine Months Ended December 31, 2025 And Other Business Matters.</t>
         </is>
       </c>
       <c r="E20" s="2" t="inlineStr">
@@ -1619,12 +1620,12 @@
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>04:03 PM</t>
+          <t>08:46 PM</t>
         </is>
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
-          <t>• Shalibhadra Finance Ltd - 511754 - Board Meeting Intimation for Intimation Of Board Meeting</t>
+          <t>• Sri Lotus Developers and Realty Ltd - 544469 - Board Meeting Intimation for Consideration Of Un-Audited (Standalone And Consolidated) Financial Results For The Quarter And Nine Months Ended December 31, 2025 And Other Business Matters</t>
         </is>
       </c>
       <c r="H20" s="3" t="inlineStr">
@@ -1634,27 +1635,27 @@
       </c>
       <c r="I20" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/7d4b194c-15a1-498b-b13a-30ad6c9a7ae9.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/e8e14be2-c7b0-4e15-957e-e52c2d394163.pdf</t>
         </is>
       </c>
     </row>
     <row r="21" ht="80" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>Go Fashion (India) Ltd</t>
+          <t>Lloyds Metals and Energy Ltd</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>543401</v>
+        <v>512455</v>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Concall Transcript</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>Go Fashion (India) Ltd - 543401 - Announcement under Regulation 30 (LODR)-Earnings Call Transcript</t>
+          <t>Lloyds Metals and Energy Ltd - 512455 - Announcement under Regulation 30 (LODR)-Investor Presentation</t>
         </is>
       </c>
       <c r="E21" s="2" t="inlineStr">
@@ -1664,12 +1665,12 @@
       </c>
       <c r="F21" s="2" t="inlineStr">
         <is>
-          <t>04:03 PM</t>
+          <t>08:45 PM</t>
         </is>
       </c>
       <c r="G21" s="2" t="inlineStr">
         <is>
-          <t>• Go Fashion (India) Ltd - 543401 - Announcement under Regulation 30 (LODR)-Earnings Call Transcript</t>
+          <t>• Lloyds Metals and Energy Ltd - 512455 - Announcement under Regulation 30 (LODR)-Investor Presentation</t>
         </is>
       </c>
       <c r="H21" s="3" t="inlineStr">
@@ -1679,27 +1680,27 @@
       </c>
       <c r="I21" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/eddf4c52-0dfe-4a10-9a02-5b41eade787b.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/a7101ae8-d26c-4f54-b4d4-3f9fe3dae5fb.pdf</t>
         </is>
       </c>
     </row>
     <row r="22" ht="80" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>Manappuram Finance Ltd</t>
+          <t>Trualt Bioenergy Ltd</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>531213</v>
+        <v>544545</v>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Concall Transcript</t>
+          <t>Board Meeting</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>Manappuram Finance Ltd - 531213 - Announcement under Regulation 30 (LODR)-Earnings Call Transcript</t>
+          <t>Trualt Bioenergy Ltd - 544545 - Board Meeting Outcome for Board Meeting Outcome For Consolidated And Standalone Unaudited Financial Results For The Quarter And Nine Months Ended December 31, 2025</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
@@ -1709,12 +1710,12 @@
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>04:03 PM</t>
+          <t>08:45 PM</t>
         </is>
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>• Manappuram Finance Ltd - 531213 - Announcement under Regulation 30 (LODR)-Earnings Call Transcript</t>
+          <t>• Trualt Bioenergy Ltd - 544545 - Board Meeting Outcome for Board Meeting Outcome For Consolidated And Standalone Unaudited Financial Results For The Quarter And Nine Months Ended December 31, 2025</t>
         </is>
       </c>
       <c r="H22" s="3" t="inlineStr">
@@ -1724,18 +1725,18 @@
       </c>
       <c r="I22" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/cd94de1e-c862-42b0-9ec1-012fd96f0d47.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/4339f522-b2bc-4e80-853d-02323bfa77a7.pdf</t>
         </is>
       </c>
     </row>
     <row r="23" ht="80" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>Genesis Ibrc India Ltd</t>
+          <t>JSW Cement Ltd</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>514336</v>
+        <v>544480</v>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
@@ -1744,7 +1745,7 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>Genesis Ibrc India Ltd - 514336 - Announcement under Regulation 30 (LODR)-Newspaper Publication</t>
+          <t>JSW Cement Ltd - 544480 - Update On Securities Purchase Agreement Under Regulation 30 And Other Applicable Provisions Of The Securities And Exchange Board Of India (Listing Obligations And Disclosure Requirements) Regulations, 2015.</t>
         </is>
       </c>
       <c r="E23" s="2" t="inlineStr">
@@ -1754,42 +1755,42 @@
       </c>
       <c r="F23" s="2" t="inlineStr">
         <is>
-          <t>04:03 PM</t>
+          <t>08:45 PM</t>
         </is>
       </c>
       <c r="G23" s="2" t="inlineStr">
         <is>
-          <t>• Genesis Ibrc India Ltd - 514336 - Announcement under Regulation 30 (LODR)-Newspaper Publication</t>
+          <t>• JSW Cement Ltd - 544480 - Update On Securities Purchase Agreement Under Regulation 30 And Other Applicable Provisions Of The Securities And Exchange Board Of India (Listing Obligations And Disclosure Requirements) Regulations, 2015</t>
         </is>
       </c>
       <c r="H23" s="3" t="inlineStr">
         <is>
-          <t>★★ NEUTRAL</t>
+          <t>★★ WATCH</t>
         </is>
       </c>
       <c r="I23" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/0796b949-4564-4488-b564-50bed68675fa.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/a1c4b75b-0d44-4319-acc6-bf80bb096692.pdf</t>
         </is>
       </c>
     </row>
     <row r="24" ht="80" customHeight="1">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>Oswal Pumps Ltd</t>
+          <t>Lloyds Metals and Energy Ltd</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>544418</v>
+        <v>512455</v>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>Investment</t>
+          <t>Board Meeting</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>Oswal Pumps Ltd - 544418 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
+          <t>Lloyds Metals and Energy Ltd - 512455 - Board Meeting Outcome for Outcome Of The Board Meeting Held On 3Rd February, 2026</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
@@ -1799,12 +1800,12 @@
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>04:03 PM</t>
+          <t>08:42 PM</t>
         </is>
       </c>
       <c r="G24" s="2" t="inlineStr">
         <is>
-          <t>• Oswal Pumps Ltd - 544418 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
+          <t>• Lloyds Metals and Energy Ltd - 512455 - Board Meeting Outcome for Outcome Of The Board Meeting Held On 3Rd February, 2026</t>
         </is>
       </c>
       <c r="H24" s="3" t="inlineStr">
@@ -1814,27 +1815,27 @@
       </c>
       <c r="I24" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/47ae0b53-a475-4f3e-a1f2-98376a82819c.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/236bb1d8-c8c7-44e2-8f7e-14023237a445.pdf</t>
         </is>
       </c>
     </row>
     <row r="25" ht="80" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>Yaan Enterprises Ltd</t>
+          <t>Tata Steel Ltd</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>538521</v>
+        <v>500470</v>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>Order Win</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>Yaan Enterprises Ltd - 538521 - Announcement under Regulation 30 (LODR)-Award_of_Order_Receipt_of_Order</t>
+          <t>Tata Steel Ltd - 500470 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
         </is>
       </c>
       <c r="E25" s="2" t="inlineStr">
@@ -1844,33 +1845,33 @@
       </c>
       <c r="F25" s="2" t="inlineStr">
         <is>
-          <t>04:02 PM</t>
+          <t>08:41 PM</t>
         </is>
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
-          <t>• Yaan Enterprises Ltd - 538521 - Announcement under Regulation 30 (LODR)-Award_of_Order_Receipt_of_Order</t>
+          <t>• Tata Steel Ltd - 500470 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
         </is>
       </c>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>★★ MODERATE POSITIVE</t>
+          <t>★★ NEUTRAL</t>
         </is>
       </c>
       <c r="I25" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/655460fb-67a8-4fda-8d37-4f452e369c8d.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/b69f25ad-9798-4a25-9270-9c57a78d7698.pdf</t>
         </is>
       </c>
     </row>
     <row r="26" ht="80" customHeight="1">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>Alfa Transformers Ltd</t>
+          <t>Adf Foods Ltd-$</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>517546</v>
+        <v>519183</v>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
@@ -1879,7 +1880,7 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>Alfa Transformers Ltd - 517546 - Announcement under Regulation 30 (LODR)-Newspaper Publication</t>
+          <t>Adf Foods Ltd-$ - 519183 - Announcement under Regulation 30 (LODR)-Change in Management</t>
         </is>
       </c>
       <c r="E26" s="2" t="inlineStr">
@@ -1889,12 +1890,12 @@
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>04:02 PM</t>
+          <t>08:41 PM</t>
         </is>
       </c>
       <c r="G26" s="2" t="inlineStr">
         <is>
-          <t>• Alfa Transformers Ltd - 517546 - Announcement under Regulation 30 (LODR)-Newspaper Publication</t>
+          <t>• Adf Foods Ltd-$ - 519183 - Announcement under Regulation 30 (LODR)-Change in Management</t>
         </is>
       </c>
       <c r="H26" s="3" t="inlineStr">
@@ -1904,27 +1905,27 @@
       </c>
       <c r="I26" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/ddf858dd-1065-4fd8-a341-369ababb2661.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/16350451-a91b-4297-ba41-fe6048a7d7a4.pdf</t>
         </is>
       </c>
     </row>
     <row r="27" ht="80" customHeight="1">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>Credo Brands Marketing Ltd</t>
+          <t>Sterling Tools Ltd-$</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>544058</v>
+        <v>530759</v>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>Investment</t>
+          <t>Financial Results</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
         <is>
-          <t>Credo Brands Marketing Ltd - 544058 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
+          <t>Sterling Tools Ltd-$ - 530759 - Financial Results For Quarter Ended 31St December 2025</t>
         </is>
       </c>
       <c r="E27" s="2" t="inlineStr">
@@ -1934,12 +1935,12 @@
       </c>
       <c r="F27" s="2" t="inlineStr">
         <is>
-          <t>04:02 PM</t>
+          <t>08:40 PM</t>
         </is>
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
-          <t>• Credo Brands Marketing Ltd - 544058 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
+          <t>• Sterling Tools Ltd-$ - 530759 - Financial Results For Quarter Ended 31St December 2025</t>
         </is>
       </c>
       <c r="H27" s="3" t="inlineStr">
@@ -1949,27 +1950,27 @@
       </c>
       <c r="I27" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/2f4ec2ff-0dd3-4f5b-89a4-67fe119ea984.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/7956a412-c476-4b39-8a1e-41725e83ca8e.pdf</t>
         </is>
       </c>
     </row>
     <row r="28" ht="80" customHeight="1">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>TCI Express Ltd</t>
+          <t>Balrampur Chini Mills Ltd</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>540212</v>
+        <v>500038</v>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>Dividend</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>TCI Express Ltd - 540212 - Record Date Of Interim Dividend I.E. Saturday, February 07, 2026.</t>
+          <t>Balrampur Chini Mills Ltd - 500038 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
         </is>
       </c>
       <c r="E28" s="2" t="inlineStr">
@@ -1979,43 +1980,42 @@
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>04:02 PM</t>
+          <t>08:39 PM</t>
         </is>
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>• TCI Express Ltd - 540212 - Record Date Of Interim Dividend I
-• Saturday, February 07, 2026</t>
-        </is>
-      </c>
-      <c r="H28" s="4" t="inlineStr">
-        <is>
-          <t>★★★ POSITIVE</t>
+          <t>• Balrampur Chini Mills Ltd - 500038 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>★★ NEUTRAL</t>
         </is>
       </c>
       <c r="I28" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/f37dc0ac-f3af-4050-836c-248734cf553b.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/c2d1ffc4-f479-45ff-889a-2e692cd31a9c.pdf</t>
         </is>
       </c>
     </row>
     <row r="29" ht="80" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>Advik Laboratories Ltd</t>
+          <t>Lloyds Metals and Energy Ltd</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>531686</v>
+        <v>512455</v>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Board Meeting</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>Advik Laboratories Ltd - 531686 - Announcement under Regulation 30 (LODR)-Newspaper Publication</t>
+          <t>Lloyds Metals and Energy Ltd - 512455 - Outcome Of Board Meeting Held On 3Rd February, 2026</t>
         </is>
       </c>
       <c r="E29" s="2" t="inlineStr">
@@ -2025,12 +2025,12 @@
       </c>
       <c r="F29" s="2" t="inlineStr">
         <is>
-          <t>04:02 PM</t>
+          <t>08:38 PM</t>
         </is>
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
-          <t>• Advik Laboratories Ltd - 531686 - Announcement under Regulation 30 (LODR)-Newspaper Publication</t>
+          <t>• Lloyds Metals and Energy Ltd - 512455 - Outcome Of Board Meeting Held On 3Rd February, 2026</t>
         </is>
       </c>
       <c r="H29" s="3" t="inlineStr">
@@ -2040,27 +2040,27 @@
       </c>
       <c r="I29" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/01eb7420-d07a-44c9-a3a4-a3d15d86c5b7.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/6ca09421-6af5-44db-b20c-443f3a2a8a9e.pdf</t>
         </is>
       </c>
     </row>
     <row r="30" ht="80" customHeight="1">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>National Fertilizers Ltd</t>
+          <t>Rossell Techsys Ltd</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>523630</v>
+        <v>544294</v>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>National Fertilizers Ltd - 523630 - Closure of Trading Window</t>
+          <t>Rossell Techsys Ltd - 544294 - Announcement under Regulation 30 (LODR)-Investor Presentation</t>
         </is>
       </c>
       <c r="E30" s="2" t="inlineStr">
@@ -2070,42 +2070,42 @@
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>04:01 PM</t>
+          <t>08:38 PM</t>
         </is>
       </c>
       <c r="G30" s="2" t="inlineStr">
         <is>
-          <t>• National Fertilizers Ltd - 523630 - Closure of Trading Window</t>
+          <t>• Rossell Techsys Ltd - 544294 - Announcement under Regulation 30 (LODR)-Investor Presentation</t>
         </is>
       </c>
       <c r="H30" s="3" t="inlineStr">
         <is>
-          <t>★★ WATCH</t>
+          <t>★★ NEUTRAL</t>
         </is>
       </c>
       <c r="I30" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/da2cabee-e640-4924-a7c8-370cc318e0b5.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/a3808d47-a3bb-47d2-aedc-1806aef355a0.pdf</t>
         </is>
       </c>
     </row>
     <row r="31" ht="80" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>Jyoti Resins &amp; Adhesives Ltd</t>
+          <t>Lumax Auto Technologies Ltd</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>514448</v>
+        <v>532796</v>
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Merger/Demerger</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>Jyoti Resins &amp; Adhesives Ltd - 514448 - Board Meeting Intimation for The Approval Of Q3 FY26 Financial Results.</t>
+          <t>Lumax Auto Technologies Ltd - 532796 - Effectiveness Of The Scheme Of Amalgamation Between Greenfuel Energy Solutions Private Limited And Lumax Resources Private Limited And Their Respective Shareholders And Creditors.</t>
         </is>
       </c>
       <c r="E31" s="2" t="inlineStr">
@@ -2115,12 +2115,12 @@
       </c>
       <c r="F31" s="2" t="inlineStr">
         <is>
-          <t>04:01 PM</t>
+          <t>08:38 PM</t>
         </is>
       </c>
       <c r="G31" s="2" t="inlineStr">
         <is>
-          <t>• Jyoti Resins &amp; Adhesives Ltd - 514448 - Board Meeting Intimation for The Approval Of Q3 FY26 Financial Results</t>
+          <t>• Lumax Auto Technologies Ltd - 532796 - Effectiveness Of The Scheme Of Amalgamation Between Greenfuel Energy Solutions Private Limited And Lumax Resources Private Limited And Their Respective Shareholders And Creditors</t>
         </is>
       </c>
       <c r="H31" s="3" t="inlineStr">
@@ -2130,27 +2130,27 @@
       </c>
       <c r="I31" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/f1583de2-8767-4ab4-8538-0cdfdb2b9fa2.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/ed12a638-9993-462e-a3d3-d83f9ad01a91.pdf</t>
         </is>
       </c>
     </row>
     <row r="32" ht="80" customHeight="1">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>Ecoboard Industries Ltd</t>
+          <t>Rashi Peripherals Ltd</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>523732</v>
+        <v>544119</v>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Board Meeting</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
         <is>
-          <t>Ecoboard Industries Ltd - 523732 - Announcement under Regulation 30 (LODR)-Newspaper Publication</t>
+          <t>Rashi Peripherals Ltd - 544119 - Board Meeting Outcome for Outcome Of Board Meeting Held On February 3, 2026.</t>
         </is>
       </c>
       <c r="E32" s="2" t="inlineStr">
@@ -2160,12 +2160,12 @@
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>04:00 PM</t>
+          <t>08:34 PM</t>
         </is>
       </c>
       <c r="G32" s="2" t="inlineStr">
         <is>
-          <t>• Ecoboard Industries Ltd - 523732 - Announcement under Regulation 30 (LODR)-Newspaper Publication</t>
+          <t>• Rashi Peripherals Ltd - 544119 - Board Meeting Outcome for Outcome Of Board Meeting Held On February 3, 2026</t>
         </is>
       </c>
       <c r="H32" s="3" t="inlineStr">
@@ -2175,27 +2175,27 @@
       </c>
       <c r="I32" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/95a3b4c3-5508-4482-8a70-9eca38752415.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/d4027588-7bae-412a-93c4-9611e8f96252.pdf</t>
         </is>
       </c>
     </row>
     <row r="33" ht="80" customHeight="1">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>PG Electroplast Ltd</t>
+          <t>NIIT Learning Systems Ltd</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>533581</v>
+        <v>543952</v>
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>Investment</t>
+          <t>Concall Transcript</t>
         </is>
       </c>
       <c r="D33" s="2" t="inlineStr">
         <is>
-          <t>PG Electroplast Ltd - 533581 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
+          <t>NIIT Learning Systems Ltd - 543952 - Announcement under Regulation 30 (LODR)-Earnings Call Transcript</t>
         </is>
       </c>
       <c r="E33" s="2" t="inlineStr">
@@ -2205,12 +2205,12 @@
       </c>
       <c r="F33" s="2" t="inlineStr">
         <is>
-          <t>03:59 PM</t>
+          <t>08:34 PM</t>
         </is>
       </c>
       <c r="G33" s="2" t="inlineStr">
         <is>
-          <t>• PG Electroplast Ltd - 533581 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
+          <t>• NIIT Learning Systems Ltd - 543952 - Announcement under Regulation 30 (LODR)-Earnings Call Transcript</t>
         </is>
       </c>
       <c r="H33" s="3" t="inlineStr">
@@ -2220,18 +2220,18 @@
       </c>
       <c r="I33" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/53e11328-04c2-49ad-84fa-72231c3550c2.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/21d2e594-cf51-4631-bc5a-f98b9b47354a.pdf</t>
         </is>
       </c>
     </row>
     <row r="34" ht="80" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>Protean eGov Technologies Ltd</t>
+          <t>Ganesha Ecosphere Ltd</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>544021</v>
+        <v>514167</v>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
@@ -2240,7 +2240,7 @@
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
-          <t>Protean eGov Technologies Ltd - 544021 - Clarification sought from Protean eGov Technologies Ltd</t>
+          <t>Ganesha Ecosphere Ltd - 514167 - Announcement Under Regulation 30 And Clause 8 Of Para B Of Part A Of SEBI (Listing Obligations And Disclosure Requirements) Regulations 2015.</t>
         </is>
       </c>
       <c r="E34" s="2" t="inlineStr">
@@ -2250,38 +2250,42 @@
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>03:59 PM</t>
+          <t>08:33 PM</t>
         </is>
       </c>
       <c r="G34" s="2" t="inlineStr">
         <is>
-          <t>• Protean eGov Technologies Ltd - 544021 - Clarification sought from Protean eGov Technologies Ltd</t>
+          <t>• Ganesha Ecosphere Ltd - 514167 - Announcement Under Regulation 30 And Clause 8 Of Para B Of Part A Of SEBI (Listing Obligations And Disclosure Requirements) Regulations 2015</t>
         </is>
       </c>
       <c r="H34" s="3" t="inlineStr">
         <is>
-          <t>★★ NEUTRAL</t>
-        </is>
-      </c>
-      <c r="I34" s="2" t="inlineStr"/>
+          <t>★★ WATCH</t>
+        </is>
+      </c>
+      <c r="I34" s="2" t="inlineStr">
+        <is>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/9d82a2c0-59bc-4f2a-a42b-9b80d60a62cf.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="80" customHeight="1">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>Kalyani Investment Company Ltd</t>
+          <t>Hari Govind International Ltd</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>533302</v>
+        <v>531971</v>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>Investment</t>
+          <t>Board Meeting</t>
         </is>
       </c>
       <c r="D35" s="2" t="inlineStr">
         <is>
-          <t>Kalyani Investment Company Ltd - 533302 - Announcement U/R 30 Of SEBI (LODR) Regulations, 2015</t>
+          <t>Hari Govind International Ltd - 531971 - Board Meeting Intimation for The Meeting To Be Held On 07Th February, 2026</t>
         </is>
       </c>
       <c r="E35" s="2" t="inlineStr">
@@ -2291,42 +2295,42 @@
       </c>
       <c r="F35" s="2" t="inlineStr">
         <is>
-          <t>03:58 PM</t>
+          <t>08:32 PM</t>
         </is>
       </c>
       <c r="G35" s="2" t="inlineStr">
         <is>
-          <t>• Kalyani Investment Company Ltd - 533302 - Announcement U/R 30 Of SEBI (LODR) Regulations, 2015</t>
+          <t>• Hari Govind International Ltd - 531971 - Board Meeting Intimation for The Meeting To Be Held On 07Th February, 2026</t>
         </is>
       </c>
       <c r="H35" s="3" t="inlineStr">
         <is>
-          <t>★★ MODERATE POSITIVE</t>
+          <t>★★ NEUTRAL</t>
         </is>
       </c>
       <c r="I35" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/3dda0b3b-3b6a-4120-bc65-954835fc5f54.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/31fca3b9-0953-4302-9821-534f0cd568ef.pdf</t>
         </is>
       </c>
     </row>
     <row r="36" ht="80" customHeight="1">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>Purple Agrotech Industries Ltd</t>
+          <t>Quess Corp Ltd</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>540159</v>
+        <v>539978</v>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>Change in Directors</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
         <is>
-          <t>Purple Agrotech Industries Ltd - 540159 - Appointment of Company Secretary and Compliance Officer</t>
+          <t>Quess Corp Ltd - 539978 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Outcome</t>
         </is>
       </c>
       <c r="E36" s="2" t="inlineStr">
@@ -2336,12 +2340,12 @@
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>03:58 PM</t>
+          <t>08:31 PM</t>
         </is>
       </c>
       <c r="G36" s="2" t="inlineStr">
         <is>
-          <t>• Purple Agrotech Industries Ltd - 540159 - Appointment of Company Secretary and Compliance Officer</t>
+          <t>• Quess Corp Ltd - 539978 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Outcome</t>
         </is>
       </c>
       <c r="H36" s="3" t="inlineStr">
@@ -2351,18 +2355,18 @@
       </c>
       <c r="I36" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/0d95cde6-783a-48c0-960f-cfb6322ca4fa.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/30ebba67-5636-4798-a64b-0da5f7c4fda1.pdf</t>
         </is>
       </c>
     </row>
     <row r="37" ht="80" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>BDH Industries Ltd</t>
+          <t>Sterling Tools Ltd-$</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>524828</v>
+        <v>530759</v>
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
@@ -2371,7 +2375,7 @@
       </c>
       <c r="D37" s="2" t="inlineStr">
         <is>
-          <t>BDH Industries Ltd - 524828 - Board Meeting Intimation for Considering And Approving The Standalone Unaudited Financial Results For The Third Quarter And Nine Months Ended On 31St December 2025 Of The Financial Year 2025-26.</t>
+          <t>Sterling Tools Ltd-$ - 530759 - Board Meeting Outcome for Outcome Of Board Meeting Held On 3Rd February, 2026</t>
         </is>
       </c>
       <c r="E37" s="2" t="inlineStr">
@@ -2381,12 +2385,12 @@
       </c>
       <c r="F37" s="2" t="inlineStr">
         <is>
-          <t>03:58 PM</t>
+          <t>08:30 PM</t>
         </is>
       </c>
       <c r="G37" s="2" t="inlineStr">
         <is>
-          <t>• BDH Industries Ltd - 524828 - Board Meeting Intimation for Considering And Approving The Standalone Unaudited Financial Results For The Third Quarter And Nine Months Ended On 31St December 2025 Of The Financial Year 2025-26</t>
+          <t>• Sterling Tools Ltd-$ - 530759 - Board Meeting Outcome for Outcome Of Board Meeting Held On 3Rd February, 2026</t>
         </is>
       </c>
       <c r="H37" s="3" t="inlineStr">
@@ -2396,27 +2400,27 @@
       </c>
       <c r="I37" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/b0178066-5adc-471e-853b-de0c5ce44d54.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/8af87a7d-e93d-4029-b71e-784aed85d5e4.pdf</t>
         </is>
       </c>
     </row>
     <row r="38" ht="80" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>MT Educare Ltd</t>
+          <t>Expleo Solutions Ltd</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>534312</v>
+        <v>533121</v>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr">
         <is>
-          <t>MT Educare Ltd - 534312 - Board Meeting Intimation for Intimation Of Board Meeting To Be Held On Wednesday, February 11Th, 2026</t>
+          <t>Expleo Solutions Ltd - 533121 - Announcement under Regulation 30 (LODR)-Press Release / Media Release</t>
         </is>
       </c>
       <c r="E38" s="2" t="inlineStr">
@@ -2426,12 +2430,12 @@
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>03:57 PM</t>
+          <t>08:30 PM</t>
         </is>
       </c>
       <c r="G38" s="2" t="inlineStr">
         <is>
-          <t>• MT Educare Ltd - 534312 - Board Meeting Intimation for Intimation Of Board Meeting To Be Held On Wednesday, February 11Th, 2026</t>
+          <t>• Expleo Solutions Ltd - 533121 - Announcement under Regulation 30 (LODR)-Press Release / Media Release</t>
         </is>
       </c>
       <c r="H38" s="3" t="inlineStr">
@@ -2441,27 +2445,27 @@
       </c>
       <c r="I38" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/b89683de-a321-442e-b5b6-a19aefc5e1a4.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/3f7d6a48-0004-4d42-a511-83a91386ed7b.pdf</t>
         </is>
       </c>
     </row>
     <row r="39" ht="80" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>Laser Diamonds Ltd</t>
+          <t>DAM Capital Advisors Ltd</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>531164</v>
+        <v>544316</v>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Financial Results</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
         <is>
-          <t>Laser Diamonds Ltd - 531164 - Board Meeting Intimation for Holding Of Board Meeting On 11Th February, 2026 For Consideration Of Unaudited Financial Results For The 3Rd Quarter Ending 31St December, 2025</t>
+          <t>DAM Capital Advisors Ltd - 544316 - Unaudited Standalone And Consolidated Financial Results For The Quarter And Nine Months Ended December 31, 2025</t>
         </is>
       </c>
       <c r="E39" s="2" t="inlineStr">
@@ -2471,12 +2475,12 @@
       </c>
       <c r="F39" s="2" t="inlineStr">
         <is>
-          <t>03:57 PM</t>
+          <t>08:28 PM</t>
         </is>
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
-          <t>• Laser Diamonds Ltd - 531164 - Board Meeting Intimation for Holding Of Board Meeting On 11Th February, 2026 For Consideration Of Unaudited Financial Results For The 3Rd Quarter Ending 31St December, 2025</t>
+          <t>• DAM Capital Advisors Ltd - 544316 - Unaudited Standalone And Consolidated Financial Results For The Quarter And Nine Months Ended December 31, 2025</t>
         </is>
       </c>
       <c r="H39" s="3" t="inlineStr">
@@ -2486,29 +2490,27 @@
       </c>
       <c r="I39" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/a6b3a0d5-ca37-4b2c-8b09-c35bab7b6b01.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/2ce8c9c1-53ab-4a34-9e7f-10725330b449.pdf</t>
         </is>
       </c>
     </row>
     <row r="40" ht="80" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>National Fertilizers Ltd</t>
+          <t>Urban Company Ltd</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>523630</v>
+        <v>544515</v>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">National Fertilizers Ltd - 523630 - Board Meeting Intimation for (A)  Intimation  Regarding  Holding  Of  Meeting  Of  Board  Of  Directors  To Consider, Approve And Take On Record Un-Audited Financial Results For The Quarter Ended 31St December, 2025.
-(B) Closure Of Trading Window For Insiders.
-</t>
+          <t>Urban Company Ltd - 544515 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
         </is>
       </c>
       <c r="E40" s="2" t="inlineStr">
@@ -2518,13 +2520,12 @@
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>03:57 PM</t>
+          <t>08:28 PM</t>
         </is>
       </c>
       <c r="G40" s="2" t="inlineStr">
         <is>
-          <t>• National Fertilizers Ltd - 523630 - Board Meeting Intimation for (A)  Intimation  Regarding  Holding  Of  Meeting  Of  Board  Of  Directors  To Consider, Approve And Take On Record Un-Audited Financial Results For The Quarter Ended 31St December, 2025
-• (B) Closure Of Trading Window For Insiders</t>
+          <t>• Urban Company Ltd - 544515 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
         </is>
       </c>
       <c r="H40" s="3" t="inlineStr">
@@ -2534,18 +2535,18 @@
       </c>
       <c r="I40" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/067794cc-3eec-4461-b632-c7e6fb1c760b.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/206a90aa-45ef-42a0-8f9d-27b259c2970c.pdf</t>
         </is>
       </c>
     </row>
     <row r="41" ht="80" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>Tata Communications Ltd</t>
+          <t>AXIS Bank Ltd</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>500483</v>
+        <v>532215</v>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
@@ -2554,7 +2555,7 @@
       </c>
       <c r="D41" s="2" t="inlineStr">
         <is>
-          <t>Tata Communications Ltd - 500483 - Announcement under Regulation 30 (LODR)-Change in Management</t>
+          <t>AXIS Bank Ltd - 532215 - Announcement under Regulation 30 (LODR)-Allotment of ESOP / ESPS</t>
         </is>
       </c>
       <c r="E41" s="2" t="inlineStr">
@@ -2564,12 +2565,12 @@
       </c>
       <c r="F41" s="2" t="inlineStr">
         <is>
-          <t>03:56 PM</t>
+          <t>08:27 PM</t>
         </is>
       </c>
       <c r="G41" s="2" t="inlineStr">
         <is>
-          <t>• Tata Communications Ltd - 500483 - Announcement under Regulation 30 (LODR)-Change in Management</t>
+          <t>• AXIS Bank Ltd - 532215 - Announcement under Regulation 30 (LODR)-Allotment of ESOP / ESPS</t>
         </is>
       </c>
       <c r="H41" s="3" t="inlineStr">
@@ -2579,27 +2580,27 @@
       </c>
       <c r="I41" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/aa287a9f-dbb6-4703-ad92-cea3f6b6330a.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/1b38d314-101f-47c4-a940-ed88e0843ddf.pdf</t>
         </is>
       </c>
     </row>
     <row r="42" ht="80" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>Premco Global Ltd-$</t>
+          <t>Hari Govind International Ltd</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>530331</v>
+        <v>531971</v>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Change in Directors</t>
         </is>
       </c>
       <c r="D42" s="2" t="inlineStr">
         <is>
-          <t>Premco Global Ltd-$ - 530331 - Board Meeting Intimation for Considering And Approving The Unaudited Financial Results (Standalone &amp; Consolidated) For The Quarter And Nine Months Ended December 31, 2025.</t>
+          <t>Hari Govind International Ltd - 531971 - Announcement under Regulation 30 (LODR)-Resignation of Director</t>
         </is>
       </c>
       <c r="E42" s="2" t="inlineStr">
@@ -2609,42 +2610,42 @@
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>03:56 PM</t>
+          <t>08:26 PM</t>
         </is>
       </c>
       <c r="G42" s="2" t="inlineStr">
         <is>
-          <t>• Premco Global Ltd-$ - 530331 - Board Meeting Intimation for Considering And Approving The Unaudited Financial Results (Standalone &amp; Consolidated) For The Quarter And Nine Months Ended December 31, 2025</t>
+          <t>• Hari Govind International Ltd - 531971 - Announcement under Regulation 30 (LODR)-Resignation of Director</t>
         </is>
       </c>
       <c r="H42" s="3" t="inlineStr">
         <is>
-          <t>★★ NEUTRAL</t>
+          <t>★★ WATCH</t>
         </is>
       </c>
       <c r="I42" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/9d250bac-c866-4d7c-8317-b46332d44fd7.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/c7a74566-842e-4be0-ac94-ceb6c619207d.pdf</t>
         </is>
       </c>
     </row>
     <row r="43" ht="80" customHeight="1">
       <c r="A43" s="2" t="inlineStr">
         <is>
-          <t>Satin Creditcare Network Ltd</t>
+          <t>NGL Fine Chem Ltd</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>539404</v>
+        <v>524774</v>
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="D43" s="2" t="inlineStr">
         <is>
-          <t>Satin Creditcare Network Ltd - 539404 - Board Meeting Outcome for Appointment Of Mr. Amit Kumar Gupta As Chief Financial Officer (Key Managerial Personnel)</t>
+          <t>NGL Fine Chem Ltd - 524774 - Disclosure under Regulation 30A of LODR</t>
         </is>
       </c>
       <c r="E43" s="2" t="inlineStr">
@@ -2654,43 +2655,42 @@
       </c>
       <c r="F43" s="2" t="inlineStr">
         <is>
-          <t>03:55 PM</t>
+          <t>08:24 PM</t>
         </is>
       </c>
       <c r="G43" s="2" t="inlineStr">
         <is>
-          <t>• Satin Creditcare Network Ltd - 539404 - Board Meeting Outcome for Appointment Of Mr
-• Amit Kumar Gupta As Chief Financial Officer (Key Managerial Personnel)</t>
+          <t>• NGL Fine Chem Ltd - 524774 - Disclosure under Regulation 30A of LODR</t>
         </is>
       </c>
       <c r="H43" s="3" t="inlineStr">
         <is>
-          <t>★★ NEUTRAL</t>
+          <t>★★ WATCH</t>
         </is>
       </c>
       <c r="I43" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/1a7476e4-a48c-4df5-851c-52cec77feb62.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/3623679a-a16e-419e-9356-76fa8d550d8b.pdf</t>
         </is>
       </c>
     </row>
     <row r="44" ht="80" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>NBCC (India) Ltd</t>
+          <t>Sical Logistics Ltd</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>534309</v>
+        <v>520086</v>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>Order Win</t>
+          <t>Board Meeting</t>
         </is>
       </c>
       <c r="D44" s="2" t="inlineStr">
         <is>
-          <t>NBCC (India) Ltd - 534309 - Intimation Of Work Orders Received By NBCC (India) Limited In The Ordinary Course Of Business Amounting To Rs. 271.32Cr. Approx.</t>
+          <t>Sical Logistics Ltd - 520086 - Intimation Regarding Postponement And Rescheduling Of Meeting Of Board Of Directors Of Sical Logistics Limited ("Company")</t>
         </is>
       </c>
       <c r="E44" s="2" t="inlineStr">
@@ -2700,42 +2700,42 @@
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>03:55 PM</t>
+          <t>08:24 PM</t>
         </is>
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
-          <t>• NBCC (India) Ltd - 534309 - Intimation Of Work Orders Received By NBCC (India) Limited In The Ordinary Course Of Business Amounting To Rs</t>
+          <t>• Sical Logistics Ltd - 520086 - Intimation Regarding Postponement And Rescheduling Of Meeting Of Board Of Directors Of Sical Logistics Limited ("Company")</t>
         </is>
       </c>
       <c r="H44" s="3" t="inlineStr">
         <is>
-          <t>★★ MODERATE POSITIVE</t>
+          <t>★★ NEUTRAL</t>
         </is>
       </c>
       <c r="I44" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/03b482f1-5917-48a3-99e0-cc3ffd46ca62.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/1711dd7b-54fc-4d15-a8fd-6c8729ee897a.pdf</t>
         </is>
       </c>
     </row>
     <row r="45" ht="80" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>Dr Agarwals Eye Hospital Ltd-$</t>
+          <t>Honasa Consumer Ltd</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>526783</v>
+        <v>544014</v>
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D45" s="2" t="inlineStr">
         <is>
-          <t>Dr Agarwals Eye Hospital Ltd-$ - 526783 - Announcement under Regulation 30 (LODR)-Change in Registered Office Address</t>
+          <t>Honasa Consumer Ltd - 544014 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
         </is>
       </c>
       <c r="E45" s="2" t="inlineStr">
@@ -2745,12 +2745,12 @@
       </c>
       <c r="F45" s="2" t="inlineStr">
         <is>
-          <t>03:54 PM</t>
+          <t>08:24 PM</t>
         </is>
       </c>
       <c r="G45" s="2" t="inlineStr">
         <is>
-          <t>• Dr Agarwals Eye Hospital Ltd-$ - 526783 - Announcement under Regulation 30 (LODR)-Change in Registered Office Address</t>
+          <t>• Honasa Consumer Ltd - 544014 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Intimation</t>
         </is>
       </c>
       <c r="H45" s="3" t="inlineStr">
@@ -2760,27 +2760,27 @@
       </c>
       <c r="I45" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/c2f5b20b-0946-42d1-8873-8affa247b5cb.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/108bb876-a6e6-459f-b683-4c72eeb9598b.pdf</t>
         </is>
       </c>
     </row>
     <row r="46" ht="80" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>BLB Ltd</t>
+          <t>Adani Ports and Special Economic Zone Ltd</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>532290</v>
+        <v>532921</v>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D46" s="2" t="inlineStr">
         <is>
-          <t>BLB Ltd - 532290 - Disclosure Under SEBI (PIT) Regulations</t>
+          <t>Adani Ports and Special Economic Zone Ltd - 532921 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Outcome</t>
         </is>
       </c>
       <c r="E46" s="2" t="inlineStr">
@@ -2790,42 +2790,42 @@
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>03:54 PM</t>
+          <t>08:23 PM</t>
         </is>
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
-          <t>• BLB Ltd - 532290 - Disclosure Under SEBI (PIT) Regulations</t>
+          <t>• Adani Ports and Special Economic Zone Ltd - 532921 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Outcome</t>
         </is>
       </c>
       <c r="H46" s="3" t="inlineStr">
         <is>
-          <t>★★ WATCH</t>
+          <t>★★ NEUTRAL</t>
         </is>
       </c>
       <c r="I46" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/cca55e22-7139-4790-82a9-e054464af1fb.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/d425e9f0-fc9f-4ac4-af8e-5f70ae87430e.pdf</t>
         </is>
       </c>
     </row>
     <row r="47" ht="80" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>DCW Ltd</t>
+          <t>Expleo Solutions Ltd</t>
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>500117</v>
+        <v>533121</v>
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>Dividend</t>
+          <t>Investment</t>
         </is>
       </c>
       <c r="D47" s="2" t="inlineStr">
         <is>
-          <t>DCW Ltd - 500117 - Corporate Action-Board to consider Dividend</t>
+          <t>Expleo Solutions Ltd - 533121 - Announcement under Regulation 30 (LODR)-Investor Presentation</t>
         </is>
       </c>
       <c r="E47" s="2" t="inlineStr">
@@ -2835,42 +2835,42 @@
       </c>
       <c r="F47" s="2" t="inlineStr">
         <is>
-          <t>03:53 PM</t>
+          <t>08:21 PM</t>
         </is>
       </c>
       <c r="G47" s="2" t="inlineStr">
         <is>
-          <t>• DCW Ltd - 500117 - Corporate Action-Board to consider Dividend</t>
-        </is>
-      </c>
-      <c r="H47" s="4" t="inlineStr">
-        <is>
-          <t>★★★ POSITIVE</t>
+          <t>• Expleo Solutions Ltd - 533121 - Announcement under Regulation 30 (LODR)-Investor Presentation</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>★★ NEUTRAL</t>
         </is>
       </c>
       <c r="I47" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/55f8e449-5ed1-414e-8b23-f8e642e0bbfc.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/32d84e67-fada-406d-9fe2-d4d6f69cd05b.pdf</t>
         </is>
       </c>
     </row>
     <row r="48" ht="80" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>Safari Industries India Ltd</t>
+          <t>Hari Govind International Ltd</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>523025</v>
+        <v>531971</v>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>Board Meeting</t>
+          <t>Change in Directors</t>
         </is>
       </c>
       <c r="D48" s="2" t="inlineStr">
         <is>
-          <t>Safari Industries India Ltd - 523025 - Board Meeting Intimation for Consideration And Approval, Amongst Other Matters For Un-Audited Standalone And Consolidated Financial Results Of The Company For The Quarter And Nine Months Ended 31St December 2025 And Raising Of Funds.</t>
+          <t>Hari Govind International Ltd - 531971 - Announcement under Regulation 30 (LODR)-Resignation of Company Secretary / Compliance Officer</t>
         </is>
       </c>
       <c r="E48" s="2" t="inlineStr">
@@ -2880,33 +2880,33 @@
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>03:53 PM</t>
+          <t>08:21 PM</t>
         </is>
       </c>
       <c r="G48" s="2" t="inlineStr">
         <is>
-          <t>• Safari Industries India Ltd - 523025 - Board Meeting Intimation for Consideration And Approval, Amongst Other Matters For Un-Audited Standalone And Consolidated Financial Results Of The Company For The Quarter And Nine Months Ended 31St December 2025 And Raising Of Funds</t>
+          <t>• Hari Govind International Ltd - 531971 - Announcement under Regulation 30 (LODR)-Resignation of Company Secretary / Compliance Officer</t>
         </is>
       </c>
       <c r="H48" s="3" t="inlineStr">
         <is>
-          <t>★★ NEUTRAL</t>
+          <t>★★ WATCH</t>
         </is>
       </c>
       <c r="I48" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/a3362c85-a648-4251-afbb-12d39f406986.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/b5f86e92-3904-4b92-a559-59adbed326e0.pdf</t>
         </is>
       </c>
     </row>
     <row r="49" ht="80" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>Kinetic Engineering Ltd</t>
+          <t>Suyog Telematics Ltd</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>500240</v>
+        <v>537259</v>
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
@@ -2915,7 +2915,7 @@
       </c>
       <c r="D49" s="2" t="inlineStr">
         <is>
-          <t>Kinetic Engineering Ltd - 500240 - Announcement under Regulation 30 (LODR)-Press Release / Media Release</t>
+          <t>Suyog Telematics Ltd - 537259 - Announcement under Regulation 30 (LODR)-Amendments to Memorandum &amp; Articles of Association</t>
         </is>
       </c>
       <c r="E49" s="2" t="inlineStr">
@@ -2925,12 +2925,12 @@
       </c>
       <c r="F49" s="2" t="inlineStr">
         <is>
-          <t>03:53 PM</t>
+          <t>08:21 PM</t>
         </is>
       </c>
       <c r="G49" s="2" t="inlineStr">
         <is>
-          <t>• Kinetic Engineering Ltd - 500240 - Announcement under Regulation 30 (LODR)-Press Release / Media Release</t>
+          <t>• Suyog Telematics Ltd - 537259 - Announcement under Regulation 30 (LODR)-Amendments to Memorandum &amp; Articles of Association</t>
         </is>
       </c>
       <c r="H49" s="3" t="inlineStr">
@@ -2940,18 +2940,18 @@
       </c>
       <c r="I49" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/22236667-bacc-43f1-9571-42faf564049a.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/d3834b35-30f6-4fa4-b827-0b562cdffc37.pdf</t>
         </is>
       </c>
     </row>
     <row r="50" ht="80" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>Abans Financial Services Ltd</t>
+          <t>V2 Retail Ltd</t>
         </is>
       </c>
       <c r="B50" s="2" t="n">
-        <v>543712</v>
+        <v>532867</v>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
@@ -2960,7 +2960,7 @@
       </c>
       <c r="D50" s="2" t="inlineStr">
         <is>
-          <t>Abans Financial Services Ltd - 543712 - Announcement under Regulation 30 (LODR)-Change in Management</t>
+          <t>V2 Retail Ltd - 532867 - Announcement under Regulation 30 (LODR)-Press Release / Media Release</t>
         </is>
       </c>
       <c r="E50" s="2" t="inlineStr">
@@ -2970,12 +2970,12 @@
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>03:52 PM</t>
+          <t>08:19 PM</t>
         </is>
       </c>
       <c r="G50" s="2" t="inlineStr">
         <is>
-          <t>• Abans Financial Services Ltd - 543712 - Announcement under Regulation 30 (LODR)-Change in Management</t>
+          <t>• V2 Retail Ltd - 532867 - Announcement under Regulation 30 (LODR)-Press Release / Media Release</t>
         </is>
       </c>
       <c r="H50" s="3" t="inlineStr">
@@ -2985,27 +2985,27 @@
       </c>
       <c r="I50" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/c26ba8bf-ef61-4754-bc10-e731897c11ee.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/d18d76b6-05ac-4ddb-abbe-00356b4703b5.pdf</t>
         </is>
       </c>
     </row>
     <row r="51" ht="80" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>PG Electroplast Ltd</t>
+          <t>DLF Ltd</t>
         </is>
       </c>
       <c r="B51" s="2" t="n">
-        <v>533581</v>
+        <v>532868</v>
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>Investment</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="D51" s="2" t="inlineStr">
         <is>
-          <t>PG Electroplast Ltd - 533581 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Outcome</t>
+          <t>DLF Ltd - 532868 - Intimation Under Regulation 30 Of The SEBI (Listing Obligations And Disclosure Requirements) Regulations, 2015</t>
         </is>
       </c>
       <c r="E51" s="2" t="inlineStr">
@@ -3015,22 +3015,22 @@
       </c>
       <c r="F51" s="2" t="inlineStr">
         <is>
-          <t>03:52 PM</t>
+          <t>08:19 PM</t>
         </is>
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
-          <t>• PG Electroplast Ltd - 533581 - Announcement under Regulation 30 (LODR)-Analyst / Investor Meet - Outcome</t>
+          <t>• DLF Ltd - 532868 - Intimation Under Regulation 30 Of The SEBI (Listing Obligations And Disclosure Requirements) Regulations, 2015</t>
         </is>
       </c>
       <c r="H51" s="3" t="inlineStr">
         <is>
-          <t>★★ NEUTRAL</t>
+          <t>★★ WATCH</t>
         </is>
       </c>
       <c r="I51" s="2" t="inlineStr">
         <is>
-          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/5545cbd4-4382-4c39-9ef9-f4beac58ebbb.pdf</t>
+          <t>https://www.bseindia.com/xml-data/corpfiling/AttachLive/3f601590-0acf-41a2-b891-b5e0df341b3e.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>